<commit_message>
Added model evaluation results
</commit_message>
<xml_diff>
--- a/attack_results.xlsx
+++ b/attack_results.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28908"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephaniedong/Documents/CS229Project/229-221-joint-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanie\Documents\229-221-joint-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="912" windowWidth="28800" windowHeight="17544"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>K-Mean Cluster Center Attacks</t>
   </si>
@@ -64,11 +64,44 @@
   <si>
     <t>Counts of Clusters</t>
   </si>
+  <si>
+    <t xml:space="preserve"> recall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> precision</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> false negatives</t>
+  </si>
+  <si>
+    <t>Logistic</t>
+  </si>
+  <si>
+    <t>1 Hidden Layer</t>
+  </si>
+  <si>
+    <t>3 Hidden Layer</t>
+  </si>
+  <si>
+    <t>5 Hidden Layer</t>
+  </si>
+  <si>
+    <t>10 Hidden Layer</t>
+  </si>
+  <si>
+    <t>Model Metrics on Validation Data</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>False Positive Rate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -961,26 +994,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BM48"/>
+  <dimension ref="A2:BM57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53:G57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" customWidth="1"/>
-    <col min="9" max="9" width="4.1640625" customWidth="1"/>
-    <col min="10" max="10" width="3.6640625" customWidth="1"/>
-    <col min="11" max="11" width="3.1640625" customWidth="1"/>
-    <col min="12" max="12" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" customWidth="1"/>
+    <col min="9" max="9" width="4.109375" customWidth="1"/>
+    <col min="10" max="10" width="4" customWidth="1"/>
+    <col min="11" max="11" width="3.109375" customWidth="1"/>
+    <col min="12" max="12" width="4.44140625" customWidth="1"/>
     <col min="13" max="39" width="4.6640625" customWidth="1"/>
     <col min="40" max="52" width="4" customWidth="1"/>
-    <col min="53" max="65" width="3.5" customWidth="1"/>
+    <col min="53" max="65" width="3.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -990,7 +1023,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1002,7 +1035,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -1014,7 +1047,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3">
         <v>1</v>
@@ -1038,7 +1071,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1064,7 +1097,7 @@
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1090,7 +1123,7 @@
         <v>0.38500000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1116,7 +1149,7 @@
         <v>0.60399999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1142,7 +1175,7 @@
         <v>0.76700000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -1168,7 +1201,7 @@
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1178,7 +1211,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>5</v>
@@ -1190,7 +1223,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3">
         <v>1</v>
@@ -1214,7 +1247,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -1240,7 +1273,7 @@
         <v>0.20200000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -1266,7 +1299,7 @@
         <v>0.32100000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -1292,7 +1325,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1318,17 +1351,17 @@
         <v>0.38590245639017401</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>1</v>
       </c>
@@ -1351,7 +1384,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1377,7 +1410,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1403,7 +1436,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1429,7 +1462,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1455,7 +1488,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1481,12 +1514,12 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>1</v>
       </c>
@@ -1509,7 +1542,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1535,7 +1568,7 @@
         <v>2844</v>
       </c>
     </row>
-    <row r="34" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -1561,7 +1594,7 @@
         <v>4504</v>
       </c>
     </row>
-    <row r="35" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -1587,7 +1620,7 @@
         <v>6037</v>
       </c>
     </row>
-    <row r="36" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -1613,7 +1646,7 @@
         <v>9167</v>
       </c>
     </row>
-    <row r="37" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1639,12 +1672,12 @@
         <v>5420</v>
       </c>
     </row>
-    <row r="40" spans="1:65" ht="24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:65" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1652,7 +1685,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1</v>
       </c>
@@ -1660,7 +1693,7 @@
         <v>2856</v>
       </c>
     </row>
-    <row r="43" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1671,7 +1704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>4</v>
       </c>
@@ -1688,7 +1721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>8</v>
       </c>
@@ -1717,7 +1750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>16</v>
       </c>
@@ -1770,7 +1803,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>32</v>
       </c>
@@ -1871,7 +1904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>64</v>
       </c>
@@ -2066,6 +2099,148 @@
       </c>
       <c r="BM48">
         <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53">
+        <v>6.6613262272682503</v>
+      </c>
+      <c r="C53">
+        <v>0.58123249299719804</v>
+      </c>
+      <c r="D53">
+        <v>0.238841794168247</v>
+      </c>
+      <c r="E53">
+        <v>0.781752488158998</v>
+      </c>
+      <c r="F53">
+        <v>2736.99775910364</v>
+      </c>
+      <c r="G53">
+        <f>1-C53</f>
+        <v>0.41876750700280196</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54">
+        <v>0.69020196750384399</v>
+      </c>
+      <c r="C54">
+        <v>0.69103641456582598</v>
+      </c>
+      <c r="D54">
+        <v>0.490495910697958</v>
+      </c>
+      <c r="E54">
+        <v>0.83313285730132203</v>
+      </c>
+      <c r="F54">
+        <v>1828.5030812324901</v>
+      </c>
+      <c r="G54">
+        <f t="shared" ref="G54:G57" si="0">1-C54</f>
+        <v>0.30896358543417402</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55">
+        <v>0.53603627344473403</v>
+      </c>
+      <c r="C55">
+        <v>0.73732492997198795</v>
+      </c>
+      <c r="D55">
+        <v>0.703700856234179</v>
+      </c>
+      <c r="E55">
+        <v>0.760432809841733</v>
+      </c>
+      <c r="F55">
+        <v>1065.7400560224</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="0"/>
+        <v>0.26267507002801205</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56">
+        <v>0.53103721742870402</v>
+      </c>
+      <c r="C56">
+        <v>0.73452380952380902</v>
+      </c>
+      <c r="D56">
+        <v>0.72523372303537903</v>
+      </c>
+      <c r="E56">
+        <v>0.742979875098423</v>
+      </c>
+      <c r="F56">
+        <v>985.60952380952301</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="0"/>
+        <v>0.26547619047619098</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57">
+        <v>0.45037841686681501</v>
+      </c>
+      <c r="C57">
+        <v>0.79782913165266101</v>
+      </c>
+      <c r="D57">
+        <v>0.77460099241646696</v>
+      </c>
+      <c r="E57">
+        <v>0.81370940976450001</v>
+      </c>
+      <c r="F57">
+        <v>810.21960784313706</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="0"/>
+        <v>0.20217086834733899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>